<commit_message>
Standardized formatting and added parameters to some parts
</commit_message>
<xml_diff>
--- a/Data/Capacitors.xlsx
+++ b/Data/Capacitors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Ceramic-0402" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7348" uniqueCount="2011">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7384" uniqueCount="2047">
   <si>
     <t>Component Type</t>
   </si>
@@ -6053,6 +6053,114 @@
   </si>
   <si>
     <t>CAPFILMSTM-0041</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0001</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0002</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0003</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0004</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0005</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0006</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0007</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0008</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0009</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0010</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0011</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0012</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0013</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0014</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0015</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0016</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0017</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0018</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0019</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0020</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0021</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0022</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0023</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0024</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0025</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0026</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0027</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0028</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0029</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0030</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0031</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0032</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0033</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0034</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0035</t>
+  </si>
+  <si>
+    <t>CAPELECPTH-0036</t>
   </si>
 </sst>
 </file>
@@ -6426,7 +6534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y59"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -15831,7 +15939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y67"/>
   <sheetViews>
-    <sheetView topLeftCell="D31" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="M3" sqref="M3:M67"/>
     </sheetView>
   </sheetViews>
@@ -18938,7 +19046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q98"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A78" sqref="A78:A98"/>
     </sheetView>
   </sheetViews>
@@ -23939,7 +24047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
@@ -23953,7 +24061,7 @@
     <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="65.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -26241,7 +26349,7 @@
   <dimension ref="A1:AC26"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28300,8 +28408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y39"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28411,6 +28519,9 @@
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2011</v>
+      </c>
       <c r="B2" t="s">
         <v>24</v>
       </c>
@@ -28440,6 +28551,9 @@
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2012</v>
+      </c>
       <c r="B3" t="s">
         <v>24</v>
       </c>
@@ -28469,6 +28583,9 @@
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2013</v>
+      </c>
       <c r="B4" t="s">
         <v>24</v>
       </c>
@@ -28498,6 +28615,9 @@
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2014</v>
+      </c>
       <c r="B5" t="s">
         <v>24</v>
       </c>
@@ -28527,6 +28647,9 @@
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2015</v>
+      </c>
       <c r="B6" t="s">
         <v>24</v>
       </c>
@@ -28556,6 +28679,9 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2016</v>
+      </c>
       <c r="B7" t="s">
         <v>24</v>
       </c>
@@ -28585,6 +28711,9 @@
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2017</v>
+      </c>
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -28614,6 +28743,9 @@
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2018</v>
+      </c>
       <c r="B9" t="s">
         <v>24</v>
       </c>
@@ -28643,6 +28775,9 @@
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2019</v>
+      </c>
       <c r="B10" t="s">
         <v>24</v>
       </c>
@@ -28672,6 +28807,9 @@
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2020</v>
+      </c>
       <c r="B11" t="s">
         <v>24</v>
       </c>
@@ -28743,6 +28881,9 @@
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2021</v>
+      </c>
       <c r="B12" t="s">
         <v>24</v>
       </c>
@@ -28814,6 +28955,9 @@
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2022</v>
+      </c>
       <c r="B13" t="s">
         <v>24</v>
       </c>
@@ -28885,6 +29029,9 @@
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2023</v>
+      </c>
       <c r="B14" t="s">
         <v>24</v>
       </c>
@@ -28914,6 +29061,9 @@
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2024</v>
+      </c>
       <c r="B15" t="s">
         <v>24</v>
       </c>
@@ -28943,6 +29093,9 @@
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2025</v>
+      </c>
       <c r="B16" t="s">
         <v>24</v>
       </c>
@@ -28971,7 +29124,10 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="17" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>2026</v>
+      </c>
       <c r="B17" t="s">
         <v>24</v>
       </c>
@@ -29001,7 +29157,10 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="18" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2027</v>
+      </c>
       <c r="B18" t="s">
         <v>24</v>
       </c>
@@ -29031,7 +29190,10 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="19" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2028</v>
+      </c>
       <c r="B19" t="s">
         <v>24</v>
       </c>
@@ -29061,7 +29223,10 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="20" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>2029</v>
+      </c>
       <c r="B20" t="s">
         <v>24</v>
       </c>
@@ -29091,7 +29256,10 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="21" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>2030</v>
+      </c>
       <c r="B21" t="s">
         <v>24</v>
       </c>
@@ -29121,7 +29289,10 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="22" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>2031</v>
+      </c>
       <c r="B22" t="s">
         <v>24</v>
       </c>
@@ -29192,7 +29363,10 @@
         <v>1631</v>
       </c>
     </row>
-    <row r="23" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2032</v>
+      </c>
       <c r="B23" t="s">
         <v>24</v>
       </c>
@@ -29263,7 +29437,10 @@
         <v>1638</v>
       </c>
     </row>
-    <row r="24" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>2033</v>
+      </c>
       <c r="B24" t="s">
         <v>24</v>
       </c>
@@ -29334,7 +29511,10 @@
         <v>1645</v>
       </c>
     </row>
-    <row r="25" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>2034</v>
+      </c>
       <c r="B25" t="s">
         <v>24</v>
       </c>
@@ -29405,7 +29585,10 @@
         <v>1653</v>
       </c>
     </row>
-    <row r="26" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>2035</v>
+      </c>
       <c r="B26" t="s">
         <v>24</v>
       </c>
@@ -29435,7 +29618,10 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="27" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>2036</v>
+      </c>
       <c r="B27" t="s">
         <v>24</v>
       </c>
@@ -29465,7 +29651,10 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="28" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>2037</v>
+      </c>
       <c r="B28" t="s">
         <v>24</v>
       </c>
@@ -29495,7 +29684,10 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="29" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>2038</v>
+      </c>
       <c r="B29" t="s">
         <v>24</v>
       </c>
@@ -29525,7 +29717,10 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="30" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>2039</v>
+      </c>
       <c r="B30" t="s">
         <v>24</v>
       </c>
@@ -29555,7 +29750,10 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="31" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>2040</v>
+      </c>
       <c r="B31" t="s">
         <v>24</v>
       </c>
@@ -29585,7 +29783,10 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="32" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>2041</v>
+      </c>
       <c r="B32" t="s">
         <v>24</v>
       </c>
@@ -29656,7 +29857,10 @@
         <v>1698</v>
       </c>
     </row>
-    <row r="33" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>2042</v>
+      </c>
       <c r="B33" t="s">
         <v>24</v>
       </c>
@@ -29727,7 +29931,10 @@
         <v>1706</v>
       </c>
     </row>
-    <row r="34" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>2043</v>
+      </c>
       <c r="B34" t="s">
         <v>24</v>
       </c>
@@ -29798,7 +30005,10 @@
         <v>1713</v>
       </c>
     </row>
-    <row r="35" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>2044</v>
+      </c>
       <c r="B35" t="s">
         <v>24</v>
       </c>
@@ -29869,7 +30079,10 @@
         <v>1721</v>
       </c>
     </row>
-    <row r="36" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>2045</v>
+      </c>
       <c r="B36" t="s">
         <v>24</v>
       </c>
@@ -29940,7 +30153,10 @@
         <v>1729</v>
       </c>
     </row>
-    <row r="37" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>2046</v>
+      </c>
       <c r="B37" t="s">
         <v>24</v>
       </c>
@@ -30011,10 +30227,10 @@
         <v>1737</v>
       </c>
     </row>
-    <row r="38" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="I39" s="2"/>
     </row>
   </sheetData>

</xml_diff>